<commit_message>
GoodInfo_v2 - 2021.11.30 完成
</commit_message>
<xml_diff>
--- a/Filter_20211130.xlsx
+++ b/Filter_20211130.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayWu\OneDrive - AAEON Technology\_OLD\Documents\Python\GoodInfo_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_93C363FDBA69C3222BCF702371D37F79A4FD5C95" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0F99448C-737F-4EBE-8737-B4B25B4AD6E8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18816" windowHeight="7968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18816" windowHeight="7968"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
   <si>
     <t>代號</t>
   </si>
@@ -391,12 +390,18 @@
   </si>
   <si>
     <t>樂士</t>
+  </si>
+  <si>
+    <t>統一超</t>
+  </si>
+  <si>
+    <t>聯光通</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -799,11 +804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1710,6 +1715,28 @@
         <v>116</v>
       </c>
       <c r="C79" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>2912</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>4903</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1733,12 +1760,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068154D9CED6A274799344D73CDDB6092" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5a2665e4f307efafdee1c9405c7148c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0" xmlns:ns4="a05e4abd-8455-4909-9372-067b8b6e3dbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb69d6d218e7dc1efa9607e3a9562cb6" ns3:_="" ns4:_="">
     <xsd:import namespace="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
@@ -1947,6 +1968,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81046D84-71BA-4494-97FE-ABE61A155419}">
   <ds:schemaRefs>
@@ -1956,23 +1983,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1E403E-48E0-45A5-8A6B-E1BE8411359D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
-    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DC88C65-3B14-4A81-80FA-D2920493807E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1989,4 +1999,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1E403E-48E0-45A5-8A6B-E1BE8411359D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>